<commit_message>
Changed incorrect rewrite rules
</commit_message>
<xml_diff>
--- a/thesis/analysis/analysis.xlsx
+++ b/thesis/analysis/analysis.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arbeit/Documents/Studium/BA/grammatical-evolution/thesis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arbeit/Documents/Studium/BA/grammatical-evolution/thesis/analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D9FB40D-1223-8C42-B86E-0AE1BAF11B0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44C61C45-7F07-544C-A3EE-FDC38B364B97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19700" activeTab="7" xr2:uid="{6ECE67CF-DEAD-C649-AB9F-F10B14D5DE84}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19700" xr2:uid="{6ECE67CF-DEAD-C649-AB9F-F10B14D5DE84}"/>
   </bookViews>
   <sheets>
     <sheet name="Tomita 1" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <sheet name="Tomita 7" sheetId="7" r:id="rId7"/>
     <sheet name="Results" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="135">
   <si>
     <t>Run</t>
   </si>
@@ -167,9 +167,6 @@
   <si>
     <t>A = epsilon|'a'C;
 C = 'b'A;</t>
-  </si>
-  <si>
-    <t>A = epsilon|'a'A;</t>
   </si>
   <si>
     <t>C = epsilon|'a'B;
@@ -598,7 +595,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -818,12 +815,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -838,12 +835,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -851,12 +842,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
@@ -880,27 +865,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
@@ -909,17 +890,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1237,8 +1233,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{748D8E23-EA8F-754C-9F4F-B2328E1EFD81}">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1255,59 +1251,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="11"/>
-      <c r="B1" s="12" t="s">
+      <c r="A1" s="9"/>
+      <c r="B1" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="13"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="31"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="4"/>
-      <c r="B2" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7" t="s">
+      <c r="B2" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="8"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="33"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="15" t="s">
+      <c r="G3" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="15" t="s">
+      <c r="H3" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="16" t="s">
+      <c r="I3" s="12" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1336,8 +1332,8 @@
       <c r="H4" s="2">
         <v>0</v>
       </c>
-      <c r="I4" s="17" t="s">
-        <v>39</v>
+      <c r="I4" s="13" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -1365,7 +1361,7 @@
       <c r="H5" s="2">
         <v>0</v>
       </c>
-      <c r="I5" s="17" t="s">
+      <c r="I5" s="13" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1394,8 +1390,8 @@
       <c r="H6" s="2">
         <v>0</v>
       </c>
-      <c r="I6" s="17" t="s">
-        <v>39</v>
+      <c r="I6" s="13" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -1423,7 +1419,7 @@
       <c r="H7" s="2">
         <v>0</v>
       </c>
-      <c r="I7" s="17" t="s">
+      <c r="I7" s="13" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1452,7 +1448,7 @@
       <c r="H8" s="2">
         <v>0</v>
       </c>
-      <c r="I8" s="17" t="s">
+      <c r="I8" s="13" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1481,7 +1477,7 @@
       <c r="H9" s="2">
         <v>0</v>
       </c>
-      <c r="I9" s="17" t="s">
+      <c r="I9" s="13" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1510,7 +1506,7 @@
       <c r="H10" s="2">
         <v>0</v>
       </c>
-      <c r="I10" s="17" t="s">
+      <c r="I10" s="13" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1539,7 +1535,7 @@
       <c r="H11" s="2">
         <v>0</v>
       </c>
-      <c r="I11" s="17" t="s">
+      <c r="I11" s="13" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1568,7 +1564,7 @@
       <c r="H12" s="2">
         <v>0</v>
       </c>
-      <c r="I12" s="17" t="s">
+      <c r="I12" s="13" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1597,8 +1593,8 @@
       <c r="H13" s="1">
         <v>0</v>
       </c>
-      <c r="I13" s="18" t="s">
-        <v>39</v>
+      <c r="I13" s="14" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -1630,7 +1626,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I14" s="9"/>
+      <c r="I14" s="7"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
@@ -1661,7 +1657,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I15" s="9"/>
+      <c r="I15" s="7"/>
     </row>
     <row r="16" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
@@ -1692,7 +1688,7 @@
         <f>ROUND(AVERAGE(H4:H13), 0)</f>
         <v>0</v>
       </c>
-      <c r="I16" s="10"/>
+      <c r="I16" s="8"/>
     </row>
     <row r="17" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
@@ -1719,7 +1715,7 @@
       <c r="H17" s="3">
         <v>0</v>
       </c>
-      <c r="I17" s="20" t="s">
+      <c r="I17" s="16" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1738,7 +1734,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E08E49A8-859D-704D-9237-0B3468A32058}">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView topLeftCell="A5" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
@@ -1756,59 +1752,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="11"/>
-      <c r="B1" s="12" t="s">
+      <c r="A1" s="9"/>
+      <c r="B1" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="13"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="31"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="4"/>
-      <c r="B2" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7" t="s">
+      <c r="B2" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="8"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="33"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="15" t="s">
+      <c r="G3" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="15" t="s">
+      <c r="H3" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="16" t="s">
+      <c r="I3" s="12" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1837,7 +1833,7 @@
       <c r="H4" s="2">
         <v>4</v>
       </c>
-      <c r="I4" s="17" t="s">
+      <c r="I4" s="13" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1866,8 +1862,8 @@
       <c r="H5" s="2">
         <v>4</v>
       </c>
-      <c r="I5" s="17" t="s">
-        <v>44</v>
+      <c r="I5" s="13" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
@@ -1895,8 +1891,8 @@
       <c r="H6" s="2">
         <v>8</v>
       </c>
-      <c r="I6" s="17" t="s">
-        <v>40</v>
+      <c r="I6" s="13" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="34" x14ac:dyDescent="0.2">
@@ -1924,8 +1920,8 @@
       <c r="H7" s="2">
         <v>6</v>
       </c>
-      <c r="I7" s="17" t="s">
-        <v>41</v>
+      <c r="I7" s="13" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="51" x14ac:dyDescent="0.2">
@@ -1953,8 +1949,8 @@
       <c r="H8" s="2">
         <v>18</v>
       </c>
-      <c r="I8" s="17" t="s">
-        <v>42</v>
+      <c r="I8" s="13" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="51" x14ac:dyDescent="0.2">
@@ -1982,7 +1978,7 @@
       <c r="H9" s="2">
         <v>7</v>
       </c>
-      <c r="I9" s="17" t="s">
+      <c r="I9" s="13" t="s">
         <v>12</v>
       </c>
     </row>
@@ -2011,8 +2007,8 @@
       <c r="H10" s="2">
         <v>5</v>
       </c>
-      <c r="I10" s="17" t="s">
-        <v>43</v>
+      <c r="I10" s="13" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="34" x14ac:dyDescent="0.2">
@@ -2040,8 +2036,8 @@
       <c r="H11" s="2">
         <v>7</v>
       </c>
-      <c r="I11" s="17" t="s">
-        <v>40</v>
+      <c r="I11" s="13" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="51" x14ac:dyDescent="0.2">
@@ -2069,7 +2065,7 @@
       <c r="H12" s="2">
         <v>8</v>
       </c>
-      <c r="I12" s="17" t="s">
+      <c r="I12" s="13" t="s">
         <v>13</v>
       </c>
     </row>
@@ -2098,7 +2094,7 @@
       <c r="H13" s="1">
         <v>8</v>
       </c>
-      <c r="I13" s="18" t="s">
+      <c r="I13" s="14" t="s">
         <v>37</v>
       </c>
     </row>
@@ -2131,7 +2127,7 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="I14" s="9"/>
+      <c r="I14" s="7"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
@@ -2162,7 +2158,7 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="I15" s="9"/>
+      <c r="I15" s="7"/>
     </row>
     <row r="16" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
@@ -2193,7 +2189,7 @@
         <f>ROUND(AVERAGE(H4:H13), 0)</f>
         <v>8</v>
       </c>
-      <c r="I16" s="10"/>
+      <c r="I16" s="8"/>
     </row>
     <row r="17" spans="1:9" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
@@ -2220,7 +2216,7 @@
       <c r="H17" s="3">
         <v>4</v>
       </c>
-      <c r="I17" s="20" t="s">
+      <c r="I17" s="16" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2259,65 +2255,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="11"/>
-      <c r="B1" s="12" t="s">
+      <c r="A1" s="9"/>
+      <c r="B1" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="13"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="31"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="4"/>
-      <c r="B2" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7" t="s">
+      <c r="B2" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="8"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="33"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="15" t="s">
+      <c r="G3" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="15" t="s">
+      <c r="H3" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="16" t="s">
+      <c r="I3" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="26"/>
-      <c r="K3" s="26"/>
-      <c r="L3" s="26"/>
-      <c r="M3" s="26"/>
     </row>
     <row r="4" spans="1:13" ht="68" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
@@ -2344,13 +2336,13 @@
       <c r="H4" s="2">
         <v>50</v>
       </c>
-      <c r="I4" s="17" t="s">
-        <v>92</v>
+      <c r="I4" s="13" t="s">
+        <v>91</v>
       </c>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
-      <c r="M4" s="25"/>
+      <c r="M4" s="21"/>
     </row>
     <row r="5" spans="1:13" ht="68" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
@@ -2377,13 +2369,13 @@
       <c r="H5" s="2">
         <v>50</v>
       </c>
-      <c r="I5" s="17" t="s">
-        <v>93</v>
+      <c r="I5" s="13" t="s">
+        <v>92</v>
       </c>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
-      <c r="M5" s="25"/>
+      <c r="M5" s="21"/>
     </row>
     <row r="6" spans="1:13" ht="68" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
@@ -2410,13 +2402,13 @@
       <c r="H6" s="2">
         <v>50</v>
       </c>
-      <c r="I6" s="17" t="s">
-        <v>94</v>
+      <c r="I6" s="13" t="s">
+        <v>93</v>
       </c>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
-      <c r="M6" s="25"/>
+      <c r="M6" s="21"/>
     </row>
     <row r="7" spans="1:13" ht="68" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
@@ -2443,13 +2435,13 @@
       <c r="H7" s="2">
         <v>50</v>
       </c>
-      <c r="I7" s="17" t="s">
-        <v>95</v>
+      <c r="I7" s="13" t="s">
+        <v>94</v>
       </c>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
-      <c r="M7" s="25"/>
+      <c r="M7" s="21"/>
     </row>
     <row r="8" spans="1:13" ht="68" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
@@ -2476,13 +2468,13 @@
       <c r="H8" s="2">
         <v>50</v>
       </c>
-      <c r="I8" s="17" t="s">
-        <v>96</v>
+      <c r="I8" s="13" t="s">
+        <v>95</v>
       </c>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
-      <c r="M8" s="25"/>
+      <c r="M8" s="21"/>
     </row>
     <row r="9" spans="1:13" ht="68" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
@@ -2509,13 +2501,13 @@
       <c r="H9" s="2">
         <v>50</v>
       </c>
-      <c r="I9" s="17" t="s">
-        <v>97</v>
+      <c r="I9" s="13" t="s">
+        <v>96</v>
       </c>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
-      <c r="M9" s="25"/>
+      <c r="M9" s="21"/>
     </row>
     <row r="10" spans="1:13" ht="68" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
@@ -2542,13 +2534,13 @@
       <c r="H10" s="2">
         <v>50</v>
       </c>
-      <c r="I10" s="17" t="s">
-        <v>98</v>
+      <c r="I10" s="13" t="s">
+        <v>97</v>
       </c>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
-      <c r="M10" s="25"/>
+      <c r="M10" s="21"/>
     </row>
     <row r="11" spans="1:13" ht="68" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
@@ -2575,13 +2567,13 @@
       <c r="H11" s="2">
         <v>50</v>
       </c>
-      <c r="I11" s="17" t="s">
-        <v>99</v>
+      <c r="I11" s="13" t="s">
+        <v>98</v>
       </c>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
-      <c r="M11" s="25"/>
+      <c r="M11" s="21"/>
     </row>
     <row r="12" spans="1:13" ht="68" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
@@ -2608,13 +2600,13 @@
       <c r="H12" s="2">
         <v>50</v>
       </c>
-      <c r="I12" s="17" t="s">
-        <v>100</v>
+      <c r="I12" s="13" t="s">
+        <v>99</v>
       </c>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
-      <c r="M12" s="25"/>
+      <c r="M12" s="21"/>
     </row>
     <row r="13" spans="1:13" ht="69" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
@@ -2641,13 +2633,13 @@
       <c r="H13" s="1">
         <v>50</v>
       </c>
-      <c r="I13" s="18" t="s">
-        <v>101</v>
+      <c r="I13" s="14" t="s">
+        <v>100</v>
       </c>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
-      <c r="M13" s="25"/>
+      <c r="M13" s="21"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
@@ -2678,11 +2670,7 @@
         <f>MAX(H4:H13)</f>
         <v>50</v>
       </c>
-      <c r="I14" s="9"/>
-      <c r="J14" s="26"/>
-      <c r="K14" s="26"/>
-      <c r="L14" s="26"/>
-      <c r="M14" s="26"/>
+      <c r="I14" s="7"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
@@ -2713,11 +2701,7 @@
         <f>MIN(H4:H13)</f>
         <v>50</v>
       </c>
-      <c r="I15" s="9"/>
-      <c r="J15" s="26"/>
-      <c r="K15" s="26"/>
-      <c r="L15" s="26"/>
-      <c r="M15" s="26"/>
+      <c r="I15" s="7"/>
     </row>
     <row r="16" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
@@ -2748,13 +2732,9 @@
         <f>ROUND(AVERAGE(H4:H13),  0)</f>
         <v>50</v>
       </c>
-      <c r="I16" s="10"/>
-      <c r="J16" s="26"/>
-      <c r="K16" s="26"/>
-      <c r="L16" s="26"/>
-      <c r="M16" s="26"/>
-    </row>
-    <row r="17" spans="1:13" ht="69" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I16" s="8"/>
+    </row>
+    <row r="17" spans="1:9" ht="69" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>10</v>
       </c>
@@ -2779,15 +2759,11 @@
       <c r="H17" s="3">
         <v>50</v>
       </c>
-      <c r="I17" s="19" t="s">
-        <v>96</v>
-      </c>
-      <c r="J17" s="26"/>
-      <c r="K17" s="26"/>
-      <c r="L17" s="26"/>
-      <c r="M17" s="26"/>
-    </row>
-    <row r="18" spans="1:13" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+      <c r="I17" s="15" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:I1"/>
@@ -2820,59 +2796,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="11"/>
-      <c r="B1" s="12" t="s">
+      <c r="A1" s="9"/>
+      <c r="B1" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="13"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="31"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="4"/>
-      <c r="B2" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7" t="s">
+      <c r="B2" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="8"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="33"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="15" t="s">
+      <c r="G3" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="15" t="s">
+      <c r="H3" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="16" t="s">
+      <c r="I3" s="12" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2883,7 +2859,7 @@
       <c r="B4" s="2">
         <v>10325</v>
       </c>
-      <c r="C4" s="21">
+      <c r="C4" s="17">
         <v>0.77600000000000002</v>
       </c>
       <c r="D4" s="2">
@@ -2895,14 +2871,14 @@
       <c r="F4" s="2">
         <v>137805</v>
       </c>
-      <c r="G4" s="21">
+      <c r="G4" s="17">
         <v>1</v>
       </c>
       <c r="H4" s="2">
         <v>14</v>
       </c>
-      <c r="I4" s="17" t="s">
-        <v>102</v>
+      <c r="I4" s="13" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="51" x14ac:dyDescent="0.2">
@@ -2912,26 +2888,26 @@
       <c r="B5" s="2">
         <v>23476</v>
       </c>
-      <c r="C5" s="21">
+      <c r="C5" s="17">
         <v>1</v>
       </c>
       <c r="D5" s="2">
         <v>48</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F5" s="2">
         <v>365513</v>
       </c>
-      <c r="G5" s="21">
+      <c r="G5" s="17">
         <v>1</v>
       </c>
       <c r="H5" s="2">
         <v>29</v>
       </c>
-      <c r="I5" s="17" t="s">
-        <v>103</v>
+      <c r="I5" s="13" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="68" x14ac:dyDescent="0.2">
@@ -2941,26 +2917,26 @@
       <c r="B6" s="2">
         <v>10985</v>
       </c>
-      <c r="C6" s="21">
+      <c r="C6" s="17">
         <v>0.85199999999999998</v>
       </c>
       <c r="D6" s="2">
         <v>50</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F6" s="2">
         <v>106093</v>
       </c>
-      <c r="G6" s="21">
+      <c r="G6" s="17">
         <v>1</v>
       </c>
       <c r="H6" s="2">
         <v>11</v>
       </c>
-      <c r="I6" s="17" t="s">
-        <v>104</v>
+      <c r="I6" s="13" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="85" x14ac:dyDescent="0.2">
@@ -2970,26 +2946,26 @@
       <c r="B7" s="2">
         <v>30101</v>
       </c>
-      <c r="C7" s="21">
+      <c r="C7" s="17">
         <v>0.99</v>
       </c>
       <c r="D7" s="2">
         <v>30</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F7" s="2">
         <v>47673</v>
       </c>
-      <c r="G7" s="21">
+      <c r="G7" s="17">
         <v>1</v>
       </c>
       <c r="H7" s="2">
         <v>7</v>
       </c>
-      <c r="I7" s="17" t="s">
-        <v>105</v>
+      <c r="I7" s="13" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="51" x14ac:dyDescent="0.2">
@@ -2999,26 +2975,26 @@
       <c r="B8" s="2">
         <v>26669</v>
       </c>
-      <c r="C8" s="21">
+      <c r="C8" s="17">
         <v>0.94399999999999995</v>
       </c>
       <c r="D8" s="2">
         <v>50</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F8" s="2">
         <v>88527</v>
       </c>
-      <c r="G8" s="21">
+      <c r="G8" s="17">
         <v>1</v>
       </c>
       <c r="H8" s="2">
         <v>10</v>
       </c>
-      <c r="I8" s="17" t="s">
-        <v>106</v>
+      <c r="I8" s="13" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="51" x14ac:dyDescent="0.2">
@@ -3028,26 +3004,26 @@
       <c r="B9" s="2">
         <v>91479</v>
       </c>
-      <c r="C9" s="21">
+      <c r="C9" s="17">
         <v>0.94399999999999995</v>
       </c>
       <c r="D9" s="2">
         <v>50</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F9" s="2">
         <v>194093</v>
       </c>
-      <c r="G9" s="21">
+      <c r="G9" s="17">
         <v>1</v>
       </c>
       <c r="H9" s="2">
         <v>17</v>
       </c>
-      <c r="I9" s="17" t="s">
-        <v>107</v>
+      <c r="I9" s="13" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="51" x14ac:dyDescent="0.2">
@@ -3057,26 +3033,26 @@
       <c r="B10" s="2">
         <v>9320</v>
       </c>
-      <c r="C10" s="21">
+      <c r="C10" s="17">
         <v>0.72499999999999998</v>
       </c>
       <c r="D10" s="2">
         <v>50</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F10" s="2">
         <v>601521</v>
       </c>
-      <c r="G10" s="21">
+      <c r="G10" s="17">
         <v>0.93</v>
       </c>
       <c r="H10" s="2">
         <v>50</v>
       </c>
-      <c r="I10" s="17" t="s">
-        <v>117</v>
+      <c r="I10" s="13" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="51" x14ac:dyDescent="0.2">
@@ -3086,26 +3062,26 @@
       <c r="B11" s="2">
         <v>9679</v>
       </c>
-      <c r="C11" s="21">
+      <c r="C11" s="17">
         <v>0.78</v>
       </c>
       <c r="D11" s="2">
         <v>50</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F11" s="2">
         <v>111527</v>
       </c>
-      <c r="G11" s="21">
+      <c r="G11" s="17">
         <v>1</v>
       </c>
       <c r="H11" s="2">
         <v>11</v>
       </c>
-      <c r="I11" s="17" t="s">
-        <v>118</v>
+      <c r="I11" s="13" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="51" x14ac:dyDescent="0.2">
@@ -3115,26 +3091,26 @@
       <c r="B12" s="2">
         <v>9530</v>
       </c>
-      <c r="C12" s="21">
+      <c r="C12" s="17">
         <v>0.78</v>
       </c>
       <c r="D12" s="2">
         <v>50</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F12" s="2">
         <v>298367</v>
       </c>
-      <c r="G12" s="21">
+      <c r="G12" s="17">
         <v>1</v>
       </c>
       <c r="H12" s="2">
         <v>24</v>
       </c>
-      <c r="I12" s="17" t="s">
-        <v>119</v>
+      <c r="I12" s="13" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="69" thickBot="1" x14ac:dyDescent="0.25">
@@ -3144,26 +3120,26 @@
       <c r="B13" s="1">
         <v>147149</v>
       </c>
-      <c r="C13" s="22">
+      <c r="C13" s="18">
         <v>0.98</v>
       </c>
       <c r="D13" s="1">
         <v>50</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F13" s="1">
         <v>51156</v>
       </c>
-      <c r="G13" s="22">
+      <c r="G13" s="18">
         <v>1</v>
       </c>
       <c r="H13" s="1">
         <v>7</v>
       </c>
-      <c r="I13" s="18" t="s">
-        <v>120</v>
+      <c r="I13" s="14" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -3174,7 +3150,7 @@
         <f>MAX(B4:B13)</f>
         <v>147149</v>
       </c>
-      <c r="C14" s="21">
+      <c r="C14" s="17">
         <f>MAX(C4:C13)</f>
         <v>1</v>
       </c>
@@ -3187,7 +3163,7 @@
         <f t="shared" ref="F14:H14" si="0">MAX(F4:F13)</f>
         <v>601521</v>
       </c>
-      <c r="G14" s="21">
+      <c r="G14" s="17">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -3195,7 +3171,7 @@
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="I14" s="9"/>
+      <c r="I14" s="7"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
@@ -3205,7 +3181,7 @@
         <f>MIN(B4:B13)</f>
         <v>9320</v>
       </c>
-      <c r="C15" s="21">
+      <c r="C15" s="17">
         <f>MIN(C4:C13)</f>
         <v>0.72499999999999998</v>
       </c>
@@ -3218,7 +3194,7 @@
         <f t="shared" ref="F15:H15" si="1">MIN(F4:F13)</f>
         <v>47673</v>
       </c>
-      <c r="G15" s="21">
+      <c r="G15" s="17">
         <f t="shared" si="1"/>
         <v>0.93</v>
       </c>
@@ -3226,7 +3202,7 @@
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="I15" s="9"/>
+      <c r="I15" s="7"/>
     </row>
     <row r="16" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
@@ -3236,7 +3212,7 @@
         <f>ROUND(AVERAGE(B4:B13),0)</f>
         <v>36871</v>
       </c>
-      <c r="C16" s="22">
+      <c r="C16" s="18">
         <f>ROUND(AVERAGE(C4:C13),3)</f>
         <v>0.877</v>
       </c>
@@ -3249,7 +3225,7 @@
         <f>ROUND(AVERAGE(F4:F13),0)</f>
         <v>200228</v>
       </c>
-      <c r="G16" s="22">
+      <c r="G16" s="18">
         <f>ROUND(AVERAGE(G4:G13),3)</f>
         <v>0.99299999999999999</v>
       </c>
@@ -3257,7 +3233,7 @@
         <f>ROUND(AVERAGE(H4:H13), 0)</f>
         <v>18</v>
       </c>
-      <c r="I16" s="10"/>
+      <c r="I16" s="8"/>
     </row>
     <row r="17" spans="1:9" ht="52" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
@@ -3273,19 +3249,19 @@
         <v>30</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F17" s="3">
         <v>298367</v>
       </c>
-      <c r="G17" s="23">
+      <c r="G17" s="19">
         <v>1</v>
       </c>
       <c r="H17" s="3">
         <v>24</v>
       </c>
-      <c r="I17" s="20" t="s">
-        <v>119</v>
+      <c r="I17" s="16" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
@@ -3321,59 +3297,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="11"/>
-      <c r="B1" s="12" t="s">
+      <c r="A1" s="9"/>
+      <c r="B1" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="13"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="31"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="4"/>
-      <c r="B2" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7" t="s">
+      <c r="B2" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="8"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="33"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="15" t="s">
+      <c r="G3" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="15" t="s">
+      <c r="H3" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="16" t="s">
+      <c r="I3" s="12" t="s">
         <v>6</v>
       </c>
     </row>
@@ -3384,7 +3360,7 @@
       <c r="B4" s="2">
         <v>25928</v>
       </c>
-      <c r="C4" s="21">
+      <c r="C4" s="17">
         <v>0.93799999999999994</v>
       </c>
       <c r="D4" s="2">
@@ -3396,14 +3372,14 @@
       <c r="F4" s="2">
         <v>452341</v>
       </c>
-      <c r="G4" s="21">
+      <c r="G4" s="17">
         <v>0.83699999999999997</v>
       </c>
       <c r="H4" s="2">
         <v>50</v>
       </c>
-      <c r="I4" s="17" t="s">
-        <v>121</v>
+      <c r="I4" s="13" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="51" x14ac:dyDescent="0.2">
@@ -3413,26 +3389,26 @@
       <c r="B5" s="2">
         <v>22480</v>
       </c>
-      <c r="C5" s="21">
+      <c r="C5" s="17">
         <v>0.94299999999999995</v>
       </c>
       <c r="D5" s="2">
         <v>50</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F5" s="2">
         <v>475529</v>
       </c>
-      <c r="G5" s="21">
+      <c r="G5" s="17">
         <v>0.93</v>
       </c>
       <c r="H5" s="2">
         <v>50</v>
       </c>
-      <c r="I5" s="17" t="s">
-        <v>122</v>
+      <c r="I5" s="13" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="51" x14ac:dyDescent="0.2">
@@ -3442,26 +3418,26 @@
       <c r="B6" s="2">
         <v>21779</v>
       </c>
-      <c r="C6" s="21">
+      <c r="C6" s="17">
         <v>0.93</v>
       </c>
       <c r="D6" s="2">
         <v>50</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F6" s="2">
         <v>474724</v>
       </c>
-      <c r="G6" s="21">
+      <c r="G6" s="17">
         <v>0.93</v>
       </c>
       <c r="H6" s="2">
         <v>50</v>
       </c>
-      <c r="I6" s="17" t="s">
-        <v>123</v>
+      <c r="I6" s="13" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="68" x14ac:dyDescent="0.2">
@@ -3471,26 +3447,26 @@
       <c r="B7" s="2">
         <v>16936</v>
       </c>
-      <c r="C7" s="21">
+      <c r="C7" s="17">
         <v>0.94</v>
       </c>
       <c r="D7" s="2">
         <v>50</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F7" s="2">
         <v>447815</v>
       </c>
-      <c r="G7" s="21">
+      <c r="G7" s="17">
         <v>0.93</v>
       </c>
       <c r="H7" s="2">
         <v>50</v>
       </c>
-      <c r="I7" s="17" t="s">
-        <v>124</v>
+      <c r="I7" s="13" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="68" x14ac:dyDescent="0.2">
@@ -3500,26 +3476,26 @@
       <c r="B8" s="2">
         <v>16280</v>
       </c>
-      <c r="C8" s="21">
+      <c r="C8" s="17">
         <v>0.93300000000000005</v>
       </c>
       <c r="D8" s="2">
         <v>50</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F8" s="2">
         <v>473058</v>
       </c>
-      <c r="G8" s="21">
+      <c r="G8" s="17">
         <v>0.86599999999999999</v>
       </c>
       <c r="H8" s="2">
         <v>50</v>
       </c>
-      <c r="I8" s="17" t="s">
-        <v>125</v>
+      <c r="I8" s="13" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="68" x14ac:dyDescent="0.2">
@@ -3529,26 +3505,26 @@
       <c r="B9" s="2">
         <v>16875</v>
       </c>
-      <c r="C9" s="21">
+      <c r="C9" s="17">
         <v>0.93300000000000005</v>
       </c>
       <c r="D9" s="2">
         <v>50</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F9" s="2">
         <v>491512</v>
       </c>
-      <c r="G9" s="21">
+      <c r="G9" s="17">
         <v>0.93</v>
       </c>
       <c r="H9" s="2">
         <v>50</v>
       </c>
-      <c r="I9" s="17" t="s">
-        <v>126</v>
+      <c r="I9" s="13" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="68" x14ac:dyDescent="0.2">
@@ -3558,26 +3534,26 @@
       <c r="B10" s="2">
         <v>18206</v>
       </c>
-      <c r="C10" s="21">
+      <c r="C10" s="17">
         <v>0.93300000000000005</v>
       </c>
       <c r="D10" s="2">
         <v>50</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F10" s="2">
         <v>439879</v>
       </c>
-      <c r="G10" s="21">
+      <c r="G10" s="17">
         <v>0.93</v>
       </c>
       <c r="H10" s="2">
         <v>50</v>
       </c>
-      <c r="I10" s="17" t="s">
-        <v>127</v>
+      <c r="I10" s="13" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="68" x14ac:dyDescent="0.2">
@@ -3587,26 +3563,26 @@
       <c r="B11" s="2">
         <v>21854</v>
       </c>
-      <c r="C11" s="21">
+      <c r="C11" s="17">
         <v>0.93300000000000005</v>
       </c>
       <c r="D11" s="2">
         <v>50</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F11" s="2">
         <v>452371</v>
       </c>
-      <c r="G11" s="21">
+      <c r="G11" s="17">
         <v>0.79100000000000004</v>
       </c>
       <c r="H11" s="2">
         <v>50</v>
       </c>
-      <c r="I11" s="17" t="s">
-        <v>128</v>
+      <c r="I11" s="13" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="51" x14ac:dyDescent="0.2">
@@ -3616,26 +3592,26 @@
       <c r="B12" s="2">
         <v>17899</v>
       </c>
-      <c r="C12" s="21">
+      <c r="C12" s="17">
         <v>0.93300000000000005</v>
       </c>
       <c r="D12" s="2">
         <v>50</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F12" s="2">
         <v>488768</v>
       </c>
-      <c r="G12" s="21">
+      <c r="G12" s="17">
         <v>0.93</v>
       </c>
       <c r="H12" s="2">
         <v>50</v>
       </c>
-      <c r="I12" s="17" t="s">
-        <v>129</v>
+      <c r="I12" s="13" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="69" thickBot="1" x14ac:dyDescent="0.25">
@@ -3645,26 +3621,26 @@
       <c r="B13" s="1">
         <v>15014</v>
       </c>
-      <c r="C13" s="22">
+      <c r="C13" s="18">
         <v>0.93600000000000005</v>
       </c>
       <c r="D13" s="1">
         <v>50</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F13" s="1">
         <v>448749</v>
       </c>
-      <c r="G13" s="22">
+      <c r="G13" s="18">
         <v>0.93</v>
       </c>
       <c r="H13" s="1">
         <v>50</v>
       </c>
-      <c r="I13" s="18" t="s">
-        <v>130</v>
+      <c r="I13" s="14" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -3675,7 +3651,7 @@
         <f>MAX(B4:B13)</f>
         <v>25928</v>
       </c>
-      <c r="C14" s="21">
+      <c r="C14" s="17">
         <f>MAX(C4:C13)</f>
         <v>0.94299999999999995</v>
       </c>
@@ -3688,7 +3664,7 @@
         <f t="shared" ref="F14:H14" si="0">MAX(F4:F13)</f>
         <v>491512</v>
       </c>
-      <c r="G14" s="21">
+      <c r="G14" s="17">
         <f t="shared" si="0"/>
         <v>0.93</v>
       </c>
@@ -3696,7 +3672,7 @@
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="I14" s="9"/>
+      <c r="I14" s="7"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
@@ -3706,7 +3682,7 @@
         <f>MIN(B4:B13)</f>
         <v>15014</v>
       </c>
-      <c r="C15" s="21">
+      <c r="C15" s="17">
         <f>MIN(C4:C13)</f>
         <v>0.93</v>
       </c>
@@ -3719,7 +3695,7 @@
         <f t="shared" ref="F15:H15" si="1">MIN(F4:F13)</f>
         <v>439879</v>
       </c>
-      <c r="G15" s="21">
+      <c r="G15" s="17">
         <f t="shared" si="1"/>
         <v>0.79100000000000004</v>
       </c>
@@ -3727,7 +3703,7 @@
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="I15" s="9"/>
+      <c r="I15" s="7"/>
     </row>
     <row r="16" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
@@ -3737,7 +3713,7 @@
         <f>ROUND(AVERAGE(B4:B13),0)</f>
         <v>19325</v>
       </c>
-      <c r="C16" s="22">
+      <c r="C16" s="18">
         <f>ROUND(AVERAGE(C4:C13),3)</f>
         <v>0.93500000000000005</v>
       </c>
@@ -3750,7 +3726,7 @@
         <f>ROUND(AVERAGE(F4:F13),0)</f>
         <v>464475</v>
       </c>
-      <c r="G16" s="22">
+      <c r="G16" s="18">
         <f>ROUND(AVERAGE(G4:G13),3)</f>
         <v>0.9</v>
       </c>
@@ -3758,7 +3734,7 @@
         <f>ROUND(AVERAGE(H4:H13), 0)</f>
         <v>50</v>
       </c>
-      <c r="I16" s="10"/>
+      <c r="I16" s="8"/>
     </row>
     <row r="17" spans="1:9" ht="52" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
@@ -3774,19 +3750,19 @@
         <v>50</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F17" s="3">
         <v>474724</v>
       </c>
-      <c r="G17" s="23">
+      <c r="G17" s="19">
         <v>0.93</v>
       </c>
       <c r="H17" s="3">
         <v>50</v>
       </c>
-      <c r="I17" s="20" t="s">
-        <v>123</v>
+      <c r="I17" s="16" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
@@ -3822,59 +3798,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="11"/>
-      <c r="B1" s="12" t="s">
+      <c r="A1" s="9"/>
+      <c r="B1" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="13"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="31"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="4"/>
-      <c r="B2" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7" t="s">
+      <c r="B2" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="8"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="33"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="15" t="s">
+      <c r="G3" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="15" t="s">
+      <c r="H3" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="16" t="s">
+      <c r="I3" s="12" t="s">
         <v>6</v>
       </c>
     </row>
@@ -3885,7 +3861,7 @@
       <c r="B4" s="2">
         <v>24319</v>
       </c>
-      <c r="C4" s="21">
+      <c r="C4" s="17">
         <v>0.77700000000000002</v>
       </c>
       <c r="D4" s="2">
@@ -3897,14 +3873,14 @@
       <c r="F4" s="2">
         <v>544244</v>
       </c>
-      <c r="G4" s="21">
+      <c r="G4" s="17">
         <v>0.79300000000000004</v>
       </c>
       <c r="H4" s="2">
         <v>50</v>
       </c>
-      <c r="I4" s="17" t="s">
-        <v>91</v>
+      <c r="I4" s="13" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="85" x14ac:dyDescent="0.2">
@@ -3914,26 +3890,26 @@
       <c r="B5" s="2">
         <v>26922</v>
       </c>
-      <c r="C5" s="21">
+      <c r="C5" s="17">
         <v>0.79300000000000004</v>
       </c>
       <c r="D5" s="2">
         <v>50</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F5" s="2">
         <v>571593</v>
       </c>
-      <c r="G5" s="21">
+      <c r="G5" s="17">
         <v>0.76300000000000001</v>
       </c>
       <c r="H5" s="2">
         <v>50</v>
       </c>
-      <c r="I5" s="17" t="s">
-        <v>108</v>
+      <c r="I5" s="13" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="51" x14ac:dyDescent="0.2">
@@ -3943,26 +3919,26 @@
       <c r="B6" s="2">
         <v>13745</v>
       </c>
-      <c r="C6" s="21">
+      <c r="C6" s="17">
         <v>0.78800000000000003</v>
       </c>
       <c r="D6" s="2">
         <v>50</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F6" s="2">
         <v>520629</v>
       </c>
-      <c r="G6" s="21">
+      <c r="G6" s="17">
         <v>0.77100000000000002</v>
       </c>
       <c r="H6" s="2">
         <v>50</v>
       </c>
-      <c r="I6" s="17" t="s">
-        <v>109</v>
+      <c r="I6" s="13" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="51" x14ac:dyDescent="0.2">
@@ -3972,26 +3948,26 @@
       <c r="B7" s="2">
         <v>12019</v>
       </c>
-      <c r="C7" s="21">
+      <c r="C7" s="17">
         <v>0.77500000000000002</v>
       </c>
       <c r="D7" s="2">
         <v>50</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F7" s="2">
         <v>525881</v>
       </c>
-      <c r="G7" s="21">
+      <c r="G7" s="17">
         <v>0.84699999999999998</v>
       </c>
       <c r="H7" s="2">
         <v>50</v>
       </c>
-      <c r="I7" s="17" t="s">
-        <v>110</v>
+      <c r="I7" s="13" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="51" x14ac:dyDescent="0.2">
@@ -4001,26 +3977,26 @@
       <c r="B8" s="2">
         <v>13380</v>
       </c>
-      <c r="C8" s="21">
+      <c r="C8" s="17">
         <v>0.76800000000000002</v>
       </c>
       <c r="D8" s="2">
         <v>50</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F8" s="2">
         <v>514690</v>
       </c>
-      <c r="G8" s="21">
+      <c r="G8" s="17">
         <v>0.77700000000000002</v>
       </c>
       <c r="H8" s="2">
         <v>50</v>
       </c>
-      <c r="I8" s="17" t="s">
-        <v>111</v>
+      <c r="I8" s="13" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="51" x14ac:dyDescent="0.2">
@@ -4030,26 +4006,26 @@
       <c r="B9" s="2">
         <v>37420</v>
       </c>
-      <c r="C9" s="21">
+      <c r="C9" s="17">
         <v>0.82599999999999996</v>
       </c>
       <c r="D9" s="2">
         <v>50</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F9" s="2">
         <v>566259</v>
       </c>
-      <c r="G9" s="21">
+      <c r="G9" s="17">
         <v>0.79300000000000004</v>
       </c>
       <c r="H9" s="2">
         <v>50</v>
       </c>
-      <c r="I9" s="17" t="s">
-        <v>112</v>
+      <c r="I9" s="13" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="51" x14ac:dyDescent="0.2">
@@ -4059,26 +4035,26 @@
       <c r="B10" s="2">
         <v>16892</v>
       </c>
-      <c r="C10" s="21">
+      <c r="C10" s="17">
         <v>0.78</v>
       </c>
       <c r="D10" s="2">
         <v>50</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F10" s="2">
         <v>543283</v>
       </c>
-      <c r="G10" s="21">
+      <c r="G10" s="17">
         <v>0.76800000000000002</v>
       </c>
       <c r="H10" s="2">
         <v>50</v>
       </c>
-      <c r="I10" s="17" t="s">
-        <v>113</v>
+      <c r="I10" s="13" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="51" x14ac:dyDescent="0.2">
@@ -4088,26 +4064,26 @@
       <c r="B11" s="2">
         <v>16193</v>
       </c>
-      <c r="C11" s="21">
+      <c r="C11" s="17">
         <v>0.78400000000000003</v>
       </c>
       <c r="D11" s="2">
         <v>50</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F11" s="2">
         <v>451692</v>
       </c>
-      <c r="G11" s="21">
+      <c r="G11" s="17">
         <v>0.73499999999999999</v>
       </c>
       <c r="H11" s="2">
         <v>50</v>
       </c>
-      <c r="I11" s="17" t="s">
-        <v>114</v>
+      <c r="I11" s="13" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="51" x14ac:dyDescent="0.2">
@@ -4117,26 +4093,26 @@
       <c r="B12" s="2">
         <v>47719</v>
       </c>
-      <c r="C12" s="21">
+      <c r="C12" s="17">
         <v>0.78900000000000003</v>
       </c>
       <c r="D12" s="2">
         <v>50</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F12" s="2">
         <v>533116</v>
       </c>
-      <c r="G12" s="21">
+      <c r="G12" s="17">
         <v>0.78800000000000003</v>
       </c>
       <c r="H12" s="2">
         <v>50</v>
       </c>
-      <c r="I12" s="17" t="s">
-        <v>115</v>
+      <c r="I12" s="13" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="52" thickBot="1" x14ac:dyDescent="0.25">
@@ -4146,26 +4122,26 @@
       <c r="B13" s="1">
         <v>10670</v>
       </c>
-      <c r="C13" s="22">
+      <c r="C13" s="18">
         <v>0.76200000000000001</v>
       </c>
       <c r="D13" s="1">
         <v>50</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F13" s="1">
         <v>559246</v>
       </c>
-      <c r="G13" s="22">
+      <c r="G13" s="18">
         <v>0.77600000000000002</v>
       </c>
       <c r="H13" s="1">
         <v>50</v>
       </c>
-      <c r="I13" s="18" t="s">
-        <v>116</v>
+      <c r="I13" s="14" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -4176,7 +4152,7 @@
         <f>MAX(B4:B13)</f>
         <v>47719</v>
       </c>
-      <c r="C14" s="21">
+      <c r="C14" s="17">
         <f>MAX(C4:C13)</f>
         <v>0.82599999999999996</v>
       </c>
@@ -4189,7 +4165,7 @@
         <f t="shared" ref="F14:H14" si="0">MAX(F4:F13)</f>
         <v>571593</v>
       </c>
-      <c r="G14" s="21">
+      <c r="G14" s="17">
         <f t="shared" si="0"/>
         <v>0.84699999999999998</v>
       </c>
@@ -4197,7 +4173,7 @@
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="I14" s="9"/>
+      <c r="I14" s="7"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
@@ -4207,7 +4183,7 @@
         <f>MIN(B4:B13)</f>
         <v>10670</v>
       </c>
-      <c r="C15" s="21">
+      <c r="C15" s="17">
         <f>MIN(C4:C13)</f>
         <v>0.76200000000000001</v>
       </c>
@@ -4220,7 +4196,7 @@
         <f t="shared" ref="F15:H15" si="1">MIN(F4:F13)</f>
         <v>451692</v>
       </c>
-      <c r="G15" s="21">
+      <c r="G15" s="17">
         <f t="shared" si="1"/>
         <v>0.73499999999999999</v>
       </c>
@@ -4228,7 +4204,7 @@
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="I15" s="9"/>
+      <c r="I15" s="7"/>
     </row>
     <row r="16" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
@@ -4238,7 +4214,7 @@
         <f>ROUND(AVERAGE(B4:B13),0)</f>
         <v>21928</v>
       </c>
-      <c r="C16" s="22">
+      <c r="C16" s="18">
         <f>ROUND(AVERAGE(C4:C13),3)</f>
         <v>0.78400000000000003</v>
       </c>
@@ -4251,7 +4227,7 @@
         <f>ROUND(AVERAGE(F4:F13),0)</f>
         <v>533063</v>
       </c>
-      <c r="G16" s="22">
+      <c r="G16" s="18">
         <f>ROUND(AVERAGE(G4:G13),3)</f>
         <v>0.78100000000000003</v>
       </c>
@@ -4259,7 +4235,7 @@
         <f>ROUND(AVERAGE(H4:H13), 0)</f>
         <v>50</v>
       </c>
-      <c r="I16" s="10"/>
+      <c r="I16" s="8"/>
     </row>
     <row r="17" spans="1:9" ht="52" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
@@ -4275,19 +4251,19 @@
         <v>50</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F17" s="3">
         <v>525881</v>
       </c>
-      <c r="G17" s="23">
+      <c r="G17" s="19">
         <v>0.84699999999999998</v>
       </c>
       <c r="H17" s="3">
         <v>50</v>
       </c>
-      <c r="I17" s="20" t="s">
-        <v>110</v>
+      <c r="I17" s="16" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
@@ -4323,59 +4299,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="11"/>
-      <c r="B1" s="12" t="s">
+      <c r="A1" s="9"/>
+      <c r="B1" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="13"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="31"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="4"/>
-      <c r="B2" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7" t="s">
+      <c r="B2" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="8"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="33"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="15" t="s">
+      <c r="G3" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="15" t="s">
+      <c r="H3" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="16" t="s">
+      <c r="I3" s="12" t="s">
         <v>6</v>
       </c>
     </row>
@@ -4386,7 +4362,7 @@
       <c r="B4" s="2">
         <v>21137</v>
       </c>
-      <c r="C4" s="21">
+      <c r="C4" s="17">
         <v>1</v>
       </c>
       <c r="D4" s="2">
@@ -4398,14 +4374,14 @@
       <c r="F4" s="2">
         <v>476585</v>
       </c>
-      <c r="G4" s="21">
+      <c r="G4" s="17">
         <v>0.91600000000000004</v>
       </c>
       <c r="H4" s="2">
         <v>50</v>
       </c>
-      <c r="I4" s="17" t="s">
-        <v>81</v>
+      <c r="I4" s="13" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="68" x14ac:dyDescent="0.2">
@@ -4415,26 +4391,26 @@
       <c r="B5" s="2">
         <v>33474</v>
       </c>
-      <c r="C5" s="21">
+      <c r="C5" s="17">
         <v>0.89200000000000002</v>
       </c>
       <c r="D5" s="2">
         <v>50</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F5" s="2">
         <v>497562</v>
       </c>
-      <c r="G5" s="21">
+      <c r="G5" s="17">
         <v>0.89700000000000002</v>
       </c>
       <c r="H5" s="2">
         <v>50</v>
       </c>
-      <c r="I5" s="17" t="s">
-        <v>82</v>
+      <c r="I5" s="13" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="68" x14ac:dyDescent="0.2">
@@ -4444,26 +4420,26 @@
       <c r="B6" s="2">
         <v>30773</v>
       </c>
-      <c r="C6" s="21">
+      <c r="C6" s="17">
         <v>0.97399999999999998</v>
       </c>
       <c r="D6" s="2">
         <v>50</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F6" s="2">
         <v>455460</v>
       </c>
-      <c r="G6" s="21">
+      <c r="G6" s="17">
         <v>0.88300000000000001</v>
       </c>
       <c r="H6" s="2">
         <v>50</v>
       </c>
-      <c r="I6" s="17" t="s">
-        <v>83</v>
+      <c r="I6" s="13" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="68" x14ac:dyDescent="0.2">
@@ -4473,26 +4449,26 @@
       <c r="B7" s="2">
         <v>22229</v>
       </c>
-      <c r="C7" s="21">
+      <c r="C7" s="17">
         <v>1</v>
       </c>
       <c r="D7" s="2">
         <v>39</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F7" s="2">
         <v>222952</v>
       </c>
-      <c r="G7" s="21">
+      <c r="G7" s="17">
         <v>1</v>
       </c>
       <c r="H7" s="2">
         <v>27</v>
       </c>
-      <c r="I7" s="17" t="s">
-        <v>84</v>
+      <c r="I7" s="13" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="85" x14ac:dyDescent="0.2">
@@ -4502,26 +4478,26 @@
       <c r="B8" s="2">
         <v>24050</v>
       </c>
-      <c r="C8" s="21">
+      <c r="C8" s="17">
         <v>0.91400000000000003</v>
       </c>
       <c r="D8" s="2">
         <v>50</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F8" s="2">
         <v>451259</v>
       </c>
-      <c r="G8" s="21">
+      <c r="G8" s="17">
         <v>0.97099999999999997</v>
       </c>
       <c r="H8" s="2">
         <v>50</v>
       </c>
-      <c r="I8" s="17" t="s">
-        <v>85</v>
+      <c r="I8" s="13" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="102" x14ac:dyDescent="0.2">
@@ -4531,26 +4507,26 @@
       <c r="B9" s="2">
         <v>24577</v>
       </c>
-      <c r="C9" s="21">
+      <c r="C9" s="17">
         <v>0.92600000000000005</v>
       </c>
       <c r="D9" s="2">
         <v>50</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F9" s="2">
         <v>467584</v>
       </c>
-      <c r="G9" s="21">
+      <c r="G9" s="17">
         <v>0.89700000000000002</v>
       </c>
       <c r="H9" s="2">
         <v>50</v>
       </c>
-      <c r="I9" s="17" t="s">
-        <v>86</v>
+      <c r="I9" s="13" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="68" x14ac:dyDescent="0.2">
@@ -4560,26 +4536,26 @@
       <c r="B10" s="2">
         <v>15460</v>
       </c>
-      <c r="C10" s="21">
+      <c r="C10" s="17">
         <v>0.995</v>
       </c>
       <c r="D10" s="2">
         <v>43</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F10" s="2">
         <v>478070</v>
       </c>
-      <c r="G10" s="21">
+      <c r="G10" s="17">
         <v>1</v>
       </c>
       <c r="H10" s="2">
         <v>49</v>
       </c>
-      <c r="I10" s="17" t="s">
-        <v>87</v>
+      <c r="I10" s="13" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="68" x14ac:dyDescent="0.2">
@@ -4589,26 +4565,26 @@
       <c r="B11" s="2">
         <v>10590</v>
       </c>
-      <c r="C11" s="21">
+      <c r="C11" s="17">
         <v>0.995</v>
       </c>
       <c r="D11" s="2">
         <v>27</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F11" s="2">
         <v>456101</v>
       </c>
-      <c r="G11" s="21">
+      <c r="G11" s="17">
         <v>0.876</v>
       </c>
       <c r="H11" s="2">
         <v>50</v>
       </c>
-      <c r="I11" s="17" t="s">
-        <v>88</v>
+      <c r="I11" s="13" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="68" x14ac:dyDescent="0.2">
@@ -4618,26 +4594,26 @@
       <c r="B12" s="2">
         <v>21918</v>
       </c>
-      <c r="C12" s="21">
+      <c r="C12" s="17">
         <v>1</v>
       </c>
       <c r="D12" s="2">
         <v>46</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F12" s="2">
         <v>410034</v>
       </c>
-      <c r="G12" s="21">
+      <c r="G12" s="17">
         <v>0.876</v>
       </c>
       <c r="H12" s="2">
         <v>50</v>
       </c>
-      <c r="I12" s="17" t="s">
-        <v>89</v>
+      <c r="I12" s="13" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="69" thickBot="1" x14ac:dyDescent="0.25">
@@ -4647,26 +4623,26 @@
       <c r="B13" s="1">
         <v>32337</v>
       </c>
-      <c r="C13" s="22">
+      <c r="C13" s="18">
         <v>0.90500000000000003</v>
       </c>
       <c r="D13" s="1">
         <v>50</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F13" s="1">
         <v>430582</v>
       </c>
-      <c r="G13" s="22">
+      <c r="G13" s="18">
         <v>0.90600000000000003</v>
       </c>
       <c r="H13" s="1">
         <v>50</v>
       </c>
-      <c r="I13" s="18" t="s">
-        <v>90</v>
+      <c r="I13" s="14" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -4677,7 +4653,7 @@
         <f>MAX(B4:B13)</f>
         <v>33474</v>
       </c>
-      <c r="C14" s="21">
+      <c r="C14" s="17">
         <f>MAX(C4:C13)</f>
         <v>1</v>
       </c>
@@ -4690,7 +4666,7 @@
         <f t="shared" ref="F14:H14" si="0">MAX(F4:F13)</f>
         <v>497562</v>
       </c>
-      <c r="G14" s="21">
+      <c r="G14" s="17">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -4698,7 +4674,7 @@
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="I14" s="9"/>
+      <c r="I14" s="7"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
@@ -4708,7 +4684,7 @@
         <f>MIN(B4:B13)</f>
         <v>10590</v>
       </c>
-      <c r="C15" s="21">
+      <c r="C15" s="17">
         <f>MIN(C4:C13)</f>
         <v>0.89200000000000002</v>
       </c>
@@ -4721,7 +4697,7 @@
         <f t="shared" ref="F15:H15" si="1">MIN(F4:F13)</f>
         <v>222952</v>
       </c>
-      <c r="G15" s="21">
+      <c r="G15" s="17">
         <f t="shared" si="1"/>
         <v>0.876</v>
       </c>
@@ -4729,7 +4705,7 @@
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="I15" s="9"/>
+      <c r="I15" s="7"/>
     </row>
     <row r="16" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
@@ -4739,7 +4715,7 @@
         <f>ROUND(AVERAGE(B4:B13),0)</f>
         <v>23655</v>
       </c>
-      <c r="C16" s="22">
+      <c r="C16" s="18">
         <f>ROUND(AVERAGE(C4:C13),3)</f>
         <v>0.96</v>
       </c>
@@ -4752,7 +4728,7 @@
         <f>ROUND(AVERAGE(F4:F13),0)</f>
         <v>434619</v>
       </c>
-      <c r="G16" s="22">
+      <c r="G16" s="18">
         <f>ROUND(AVERAGE(G4:G13),3)</f>
         <v>0.92200000000000004</v>
       </c>
@@ -4760,7 +4736,7 @@
         <f>ROUND(AVERAGE(H4:H13), 0)</f>
         <v>48</v>
       </c>
-      <c r="I16" s="10"/>
+      <c r="I16" s="8"/>
     </row>
     <row r="17" spans="1:9" ht="69" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
@@ -4769,26 +4745,26 @@
       <c r="B17" s="3">
         <v>22229</v>
       </c>
-      <c r="C17" s="23">
+      <c r="C17" s="19">
         <v>1</v>
       </c>
       <c r="D17" s="3">
         <v>39</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F17" s="3">
         <v>478070</v>
       </c>
-      <c r="G17" s="23">
+      <c r="G17" s="19">
         <v>1</v>
       </c>
       <c r="H17" s="3">
         <v>49</v>
       </c>
-      <c r="I17" s="20" t="s">
-        <v>87</v>
+      <c r="I17" s="16" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
@@ -4806,7 +4782,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50552819-AF47-C745-BCED-E75DE5E4DF2C}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="143" workbookViewId="0">
+    <sheetView zoomScale="143" workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
@@ -4824,46 +4800,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="27"/>
-      <c r="B1" s="28" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="12" t="s">
+      <c r="A1" s="22"/>
+      <c r="B1" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="13"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="31"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="B2" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="C2" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="D2" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="D2" s="15" t="s">
-        <v>134</v>
-      </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="G2" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="H2" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="H2" s="15" t="s">
-        <v>134</v>
-      </c>
-      <c r="I2" s="16" t="s">
+      <c r="I2" s="12" t="s">
         <v>10</v>
       </c>
     </row>
@@ -4875,15 +4851,15 @@
         <f>'Tomita 1'!$B$16</f>
         <v>150</v>
       </c>
-      <c r="C3" s="21">
+      <c r="C3" s="17">
         <f>'Tomita 1'!C$16</f>
         <v>1</v>
       </c>
-      <c r="D3" s="24">
+      <c r="D3" s="20">
         <f>'Tomita 1'!D$16</f>
         <v>0</v>
       </c>
-      <c r="E3" s="34" t="str">
+      <c r="E3" s="28" t="str">
         <f>'Tomita 1'!E$17</f>
         <v>a*</v>
       </c>
@@ -4899,7 +4875,7 @@
         <f>'Tomita 1'!H$16</f>
         <v>0</v>
       </c>
-      <c r="I3" s="25" t="str">
+      <c r="I3" s="21" t="str">
         <f>'Tomita 1'!I$17</f>
         <v>A = 'a'A | epsilon;</v>
       </c>
@@ -4912,15 +4888,15 @@
         <f>'Tomita 2'!$B$16</f>
         <v>108</v>
       </c>
-      <c r="C4" s="21">
+      <c r="C4" s="17">
         <f>'Tomita 2'!C$16</f>
         <v>1</v>
       </c>
-      <c r="D4" s="24">
+      <c r="D4" s="20">
         <f>'Tomita 2'!D$16</f>
         <v>0</v>
       </c>
-      <c r="E4" s="34" t="str">
+      <c r="E4" s="28" t="str">
         <f>'Tomita 2'!E$17</f>
         <v>(ab)*</v>
       </c>
@@ -4936,7 +4912,7 @@
         <f>'Tomita 2'!H$16</f>
         <v>8</v>
       </c>
-      <c r="I4" s="25" t="str">
+      <c r="I4" s="21" t="str">
         <f>'Tomita 2'!I$17</f>
         <v>A = epsilon|'a'C;
 C = 'b'A;</v>
@@ -4950,15 +4926,15 @@
         <f>'Tomita 3'!$B$16</f>
         <v>204332</v>
       </c>
-      <c r="C5" s="21">
+      <c r="C5" s="17">
         <f>'Tomita 3'!C$16</f>
         <v>0.88700000000000001</v>
       </c>
-      <c r="D5" s="24">
+      <c r="D5" s="20">
         <f>'Tomita 3'!D$16</f>
         <v>50</v>
       </c>
-      <c r="E5" s="34" t="str">
+      <c r="E5" s="28" t="str">
         <f>'Tomita 3'!E$17</f>
         <v>((((b(((b((b(b|a))|a)*)|((b((b((b(b((b(b|a))|b)))|b))|b))|a)*)|b))|a)|b)|((b|a)|((b(b|(b(b((ba)|b)))))|a)*))</v>
       </c>
@@ -4974,7 +4950,7 @@
         <f>'Tomita 3'!H$16</f>
         <v>50</v>
       </c>
-      <c r="I5" s="25" t="str">
+      <c r="I5" s="21" t="str">
         <f>'Tomita 3'!I$17</f>
         <v>A = epsilon|'a'C|'a'|'b'A|'b'D;
 D = 'b';
@@ -4990,15 +4966,15 @@
         <f>'Tomita 4'!$B$16</f>
         <v>36871</v>
       </c>
-      <c r="C6" s="21">
+      <c r="C6" s="17">
         <f>'Tomita 4'!C$16</f>
         <v>0.877</v>
       </c>
-      <c r="D6" s="24">
+      <c r="D6" s="20">
         <f>'Tomita 4'!D$16</f>
         <v>48</v>
       </c>
-      <c r="E6" s="34" t="str">
+      <c r="E6" s="28" t="str">
         <f>'Tomita 4'!E$17</f>
         <v>((a+|((((((b(b|a))|b)a)|a)*b?)b?))(a*|((((b|(a|b))|a)|b)a)))</v>
       </c>
@@ -5014,7 +4990,7 @@
         <f>'Tomita 4'!H$16</f>
         <v>18</v>
       </c>
-      <c r="I6" s="25" t="str">
+      <c r="I6" s="21" t="str">
         <f>'Tomita 4'!I$17</f>
         <v>A = 'a'A|epsilon|'b'C|'b'B;
 C = 'a'A|epsilon|'a';
@@ -5029,15 +5005,15 @@
         <f>'Tomita 5'!$B$16</f>
         <v>19325</v>
       </c>
-      <c r="C7" s="21">
+      <c r="C7" s="17">
         <f>'Tomita 5'!C$16</f>
         <v>0.93500000000000005</v>
       </c>
-      <c r="D7" s="24">
+      <c r="D7" s="20">
         <f>'Tomita 5'!D$16</f>
         <v>50</v>
       </c>
-      <c r="E7" s="34" t="str">
+      <c r="E7" s="28" t="str">
         <f>'Tomita 5'!E$17</f>
         <v>((b|(((a|b)|a)(((b|((b|a)|((b|a)|((ab)b))))|a)((b|a)|((ab)b)))))((b|a)|(a|b)))*</v>
       </c>
@@ -5053,7 +5029,7 @@
         <f>'Tomita 5'!H$16</f>
         <v>50</v>
       </c>
-      <c r="I7" s="25" t="str">
+      <c r="I7" s="21" t="str">
         <f>'Tomita 5'!I$17</f>
         <v>B = epsilon|'b'D|'a'D;
 D = 'a'B|'b'B;
@@ -5068,15 +5044,15 @@
         <f>'Tomita 6'!$B$16</f>
         <v>21928</v>
       </c>
-      <c r="C8" s="21">
+      <c r="C8" s="17">
         <f>'Tomita 6'!C$16</f>
         <v>0.78400000000000003</v>
       </c>
-      <c r="D8" s="24">
+      <c r="D8" s="20">
         <f>'Tomita 6'!D$16</f>
         <v>50</v>
       </c>
-      <c r="E8" s="34" t="str">
+      <c r="E8" s="28" t="str">
         <f>'Tomita 6'!E$17</f>
         <v>((((b((((a|b)|(((b(b|a))|a)|(a|((b(b|a))b))))((b(b|a))|a))(((b(b|a))(a|b))|a)))(b|a))(ab))*|((((((b|(((ab)(a|((((b(b|a))(b|a))|a)|b)))((b|a)|b)))|((b|a)a))((ab)|a)*)|(((((((b(b|a))(b|a))|(b|a))|b)((b(b|a))|a))|(b|a))((b(b|a))|a)))((b(b|((ab)(a|b))))|a))((b(b|a))|a)*))</v>
       </c>
@@ -5092,7 +5068,7 @@
         <f>'Tomita 6'!H$16</f>
         <v>50</v>
       </c>
-      <c r="I8" s="25" t="str">
+      <c r="I8" s="21" t="str">
         <f>'Tomita 6'!I$17</f>
         <v>C = 'a'B|epsilon|'a'|'b'A;
 A = 'a'C|'b'B;
@@ -5100,38 +5076,38 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="68" x14ac:dyDescent="0.2">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="14">
+      <c r="B9" s="10">
         <f>'Tomita 7'!$B$16</f>
         <v>23655</v>
       </c>
-      <c r="C9" s="21">
+      <c r="C9" s="17">
         <f>'Tomita 7'!C$16</f>
         <v>0.96</v>
       </c>
-      <c r="D9" s="24">
+      <c r="D9" s="20">
         <f>'Tomita 7'!D$16</f>
         <v>44</v>
       </c>
-      <c r="E9" s="34" t="str">
+      <c r="E9" s="28" t="str">
         <f>'Tomita 7'!E$17</f>
         <v>(((b(((a+|b*)|(a|b))|(b*a+)))|(a+|b*))(a?(((b*(b|a)?)a*)|(a|(b|a)))))</v>
       </c>
-      <c r="F9" s="15">
+      <c r="F9" s="11">
         <f>'Tomita 7'!F$16</f>
         <v>434619</v>
       </c>
-      <c r="G9" s="15">
+      <c r="G9" s="11">
         <f>'Tomita 7'!G$16</f>
         <v>0.92200000000000004</v>
       </c>
-      <c r="H9" s="15">
+      <c r="H9" s="11">
         <f>'Tomita 7'!H$16</f>
         <v>48</v>
       </c>
-      <c r="I9" s="35" t="str">
+      <c r="I9" s="29" t="str">
         <f>'Tomita 7'!I$17</f>
         <v>A = 'a'B|epsilon|'b'C|'b'B|'a'|'b'A|'a'D;
 B = 'a'B|epsilon|'b'C|'a'|'b'D|'a'D;
@@ -5140,35 +5116,35 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="29" t="s">
-        <v>135</v>
-      </c>
-      <c r="B10" s="30">
+      <c r="A10" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="B10" s="24">
         <f>ROUND(AVERAGE(B3:B9),0)</f>
         <v>43767</v>
       </c>
-      <c r="C10" s="32">
+      <c r="C10" s="26">
         <f>ROUND(AVERAGE(C3:C9),3)</f>
         <v>0.92</v>
       </c>
-      <c r="D10" s="33">
+      <c r="D10" s="27">
         <f>ROUND(AVERAGE(D3:D9),0)</f>
         <v>35</v>
       </c>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30">
-        <f t="shared" ref="C10:I10" si="0">ROUND(AVERAGE(F3:F9),0)</f>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24">
+        <f t="shared" ref="F10:H10" si="0">ROUND(AVERAGE(F3:F9),0)</f>
         <v>518245</v>
       </c>
-      <c r="G10" s="30">
+      <c r="G10" s="24">
         <f>ROUND(AVERAGE(G3:G9),3)</f>
         <v>0.92600000000000005</v>
       </c>
-      <c r="H10" s="30">
+      <c r="H10" s="24">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="I10" s="31"/>
+      <c r="I10" s="25"/>
     </row>
     <row r="11" spans="1:9" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>

</xml_diff>